<commit_message>
#50 modify xlsx file
</commit_message>
<xml_diff>
--- a/testcase/real.xlsx
+++ b/testcase/real.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39D4A5F-276A-D94E-B94A-2E686650CB80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85127873-877A-B14A-BE63-06E9369AF954}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16960" yWindow="0" windowWidth="16640" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16960" yWindow="0" windowWidth="16640" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="186">
   <si>
     <t>username</t>
   </si>
@@ -673,6 +673,14 @@
   </si>
   <si>
     <t>学生认真学习，很好</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>teacherCommitted</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newcomerCommitted</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1089,7 +1097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="P2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
@@ -2754,10 +2762,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:G2"/>
+  <dimension ref="B1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2769,7 +2777,7 @@
     <col min="7" max="7" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1">
+    <row r="1" spans="2:9" s="1" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2788,8 +2796,14 @@
       <c r="G1" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="2:7">
+      <c r="H1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9">
       <c r="B2" t="s">
         <v>128</v>
       </c>
@@ -2807,6 +2821,12 @@
       </c>
       <c r="G2" t="s">
         <v>183</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#52 now latency test is added, resluts ok, but not added to unittest because it takes long time for write db, modify real.xlsx
</commit_message>
<xml_diff>
--- a/testcase/real.xlsx
+++ b/testcase/real.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85127873-877A-B14A-BE63-06E9369AF954}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B13703-DC2B-B44E-BA04-704DDF15F6C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16960" yWindow="0" windowWidth="16640" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16960" yWindow="0" windowWidth="26180" windowHeight="21200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="185">
   <si>
     <t>username</t>
   </si>
@@ -299,10 +299,6 @@
   </si>
   <si>
     <t>学习未通过</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1097,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB16"/>
   <sheetViews>
-    <sheetView topLeftCell="P2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1187,7 +1183,7 @@
         <v>17</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>18</v>
@@ -1219,25 +1215,25 @@
     </row>
     <row r="2" spans="1:28">
       <c r="A2" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>80</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>77</v>
@@ -1249,7 +1245,7 @@
         <v>68</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>72</v>
@@ -1267,13 +1263,13 @@
         <v>1</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="U2" s="4">
         <v>0</v>
@@ -1282,45 +1278,45 @@
         <v>78</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>78</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z2" s="4" t="s">
         <v>78</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:28">
       <c r="A3" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>81</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>77</v>
@@ -1332,7 +1328,7 @@
         <v>68</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>77</v>
@@ -1350,13 +1346,13 @@
         <v>1</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>77</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U3" s="4">
         <v>0</v>
@@ -1365,45 +1361,45 @@
         <v>0</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X3" s="4" t="s">
         <v>72</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z3" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA3" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AB3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:28">
       <c r="A4" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>82</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>77</v>
@@ -1415,10 +1411,10 @@
         <v>68</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>71</v>
@@ -1433,13 +1429,13 @@
         <v>1</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U4" s="4">
         <v>0</v>
@@ -1448,45 +1444,45 @@
         <v>0</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X4" s="4" t="s">
         <v>78</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z4" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA4" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AB4" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:28">
       <c r="A5" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>77</v>
@@ -1501,7 +1497,7 @@
         <v>73</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>71</v>
@@ -1516,13 +1512,13 @@
         <v>1</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U5" s="4">
         <v>0</v>
@@ -1531,45 +1527,45 @@
         <v>0</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB5" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="Y5" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA5" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="AB5" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:28">
       <c r="A6" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>82</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>77</v>
@@ -1581,7 +1577,7 @@
         <v>68</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>72</v>
@@ -1599,13 +1595,13 @@
         <v>1</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S6" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U6" s="4">
         <v>0</v>
@@ -1614,57 +1610,57 @@
         <v>0</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X6" s="4" t="s">
         <v>78</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z6" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA6" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AB6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:28">
       <c r="A7" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>77</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>68</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>77</v>
@@ -1682,13 +1678,13 @@
         <v>1</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S7" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U7" s="4">
         <v>0</v>
@@ -1697,19 +1693,19 @@
         <v>0</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X7" s="4" t="s">
         <v>72</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z7" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA7" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AB7" s="4">
         <v>5</v>
@@ -1717,31 +1713,31 @@
     </row>
     <row r="8" spans="1:28">
       <c r="A8" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>77</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>68</v>
@@ -1750,7 +1746,7 @@
         <v>74</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>71</v>
@@ -1765,13 +1761,13 @@
         <v>1</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S8" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U8" s="4">
         <v>0</v>
@@ -1780,19 +1776,19 @@
         <v>0</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X8" s="4" t="s">
         <v>72</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z8" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA8" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AB8" s="4">
         <v>5</v>
@@ -1800,40 +1796,40 @@
     </row>
     <row r="9" spans="1:28">
       <c r="A9" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>77</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>68</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>71</v>
@@ -1848,13 +1844,13 @@
         <v>1</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U9" s="4">
         <v>0</v>
@@ -1863,19 +1859,19 @@
         <v>0</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X9" s="4" t="s">
         <v>71</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z9" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA9" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AB9" s="4">
         <v>5</v>
@@ -1883,25 +1879,25 @@
     </row>
     <row r="10" spans="1:28">
       <c r="A10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>77</v>
@@ -1913,7 +1909,7 @@
         <v>68</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>72</v>
@@ -1931,13 +1927,13 @@
         <v>1</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S10" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U10" s="4">
         <v>0</v>
@@ -1946,19 +1942,19 @@
         <v>0</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X10" s="4" t="s">
         <v>71</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z10" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA10" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AB10" s="4">
         <v>5</v>
@@ -1966,25 +1962,25 @@
     </row>
     <row r="11" spans="1:28">
       <c r="A11" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>77</v>
@@ -2014,13 +2010,13 @@
         <v>1</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S11" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U11" s="4">
         <v>0</v>
@@ -2029,19 +2025,19 @@
         <v>0</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X11" s="4" t="s">
         <v>71</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z11" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA11" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AB11" s="4">
         <v>5</v>
@@ -2049,25 +2045,25 @@
     </row>
     <row r="12" spans="1:28">
       <c r="A12" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>77</v>
@@ -2079,10 +2075,10 @@
         <v>68</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>71</v>
@@ -2097,13 +2093,13 @@
         <v>1</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S12" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U12" s="4">
         <v>0</v>
@@ -2112,19 +2108,19 @@
         <v>0</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X12" s="4" t="s">
         <v>71</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z12" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA12" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AB12" s="4">
         <v>5</v>
@@ -2138,19 +2134,19 @@
         <v>79</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>78</v>
@@ -2159,10 +2155,10 @@
         <v>70</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>78</v>
@@ -2177,13 +2173,13 @@
         <v>78</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S13" s="4" t="s">
         <v>77</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U13" s="4" t="s">
         <v>72</v>
@@ -2192,19 +2188,19 @@
         <v>72</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X13" s="4" t="s">
         <v>78</v>
       </c>
       <c r="Y13" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z13" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA13" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AB13" s="4" t="s">
         <v>78</v>
@@ -2212,25 +2208,25 @@
     </row>
     <row r="14" spans="1:28">
       <c r="A14" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>78</v>
@@ -2257,13 +2253,13 @@
         <v>78</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S14" s="4" t="s">
         <v>77</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="U14" s="4" t="s">
         <v>72</v>
@@ -2272,19 +2268,19 @@
         <v>72</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X14" s="4" t="s">
         <v>78</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Z14" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA14" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AB14" s="4" t="s">
         <v>78</v>
@@ -2292,25 +2288,25 @@
     </row>
     <row r="15" spans="1:28">
       <c r="A15" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>78</v>
@@ -2319,7 +2315,7 @@
         <v>70</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>77</v>
@@ -2337,13 +2333,13 @@
         <v>78</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S15" s="4" t="s">
         <v>77</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="U15" s="4" t="s">
         <v>72</v>
@@ -2352,19 +2348,19 @@
         <v>72</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X15" s="4" t="s">
         <v>78</v>
       </c>
       <c r="Y15" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Z15" s="4" t="s">
         <v>78</v>
       </c>
       <c r="AA15" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AB15" s="4" t="s">
         <v>78</v>
@@ -2372,25 +2368,25 @@
     </row>
     <row r="16" spans="1:28">
       <c r="A16" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>78</v>
@@ -2399,10 +2395,10 @@
         <v>70</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>72</v>
@@ -2417,13 +2413,13 @@
         <v>78</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S16" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U16" s="4" t="s">
         <v>72</v>
@@ -2432,19 +2428,19 @@
         <v>72</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X16" s="4" t="s">
         <v>72</v>
       </c>
       <c r="Y16" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Z16" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA16" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AB16" s="4" t="s">
         <v>78</v>
@@ -2569,7 +2565,7 @@
         <v>62</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>66</v>
@@ -2693,10 +2689,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="2:5">
@@ -2704,10 +2700,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -2715,10 +2711,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="2:5">
@@ -2729,7 +2725,7 @@
         <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="2:5">
@@ -2740,7 +2736,7 @@
         <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="2:5">
@@ -2751,7 +2747,7 @@
         <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2764,7 +2760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -2797,30 +2793,30 @@
         <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="2" spans="2:9">
       <c r="B2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F2">
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -2892,7 +2888,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -2922,7 +2918,7 @@
         <v>44</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -2930,19 +2926,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G2" s="4">
         <v>400</v>
@@ -2951,7 +2947,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>78</v>
@@ -2962,19 +2958,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>178</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G3" s="4">
         <v>4000</v>
@@ -2983,7 +2979,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>78</v>
@@ -3015,7 +3011,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -3069,7 +3065,7 @@
         <v>53</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -3096,7 +3092,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -3141,7 +3137,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>54</v>
@@ -3189,7 +3185,7 @@
         <v>35</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#49 add new write db function for new tables
</commit_message>
<xml_diff>
--- a/testcase/real.xlsx
+++ b/testcase/real.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B13703-DC2B-B44E-BA04-704DDF15F6C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B62680-656F-EC4D-BEA1-B0B564B8B0CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16960" yWindow="0" windowWidth="26180" windowHeight="21200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="18000" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,19 @@
     <sheet name="userprogramtable" sheetId="10" r:id="rId10"/>
     <sheet name="usercontenttable" sheetId="11" r:id="rId11"/>
     <sheet name="userlessontable" sheetId="12" r:id="rId12"/>
+    <sheet name="notificationtable" sheetId="19" r:id="rId13"/>
+    <sheet name="grouptable" sheetId="20" r:id="rId14"/>
+    <sheet name="usernotificationtable" sheetId="21" r:id="rId15"/>
+    <sheet name="usergrouptable" sheetId="22" r:id="rId16"/>
+    <sheet name="userscheduledtable" sheetId="23" r:id="rId17"/>
+    <sheet name="schedulednotificationtable" sheetId="24" r:id="rId18"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="197">
   <si>
     <t>username</t>
   </si>
@@ -678,13 +684,52 @@
   <si>
     <t>newcomerCommitted</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>author_role</t>
+  </si>
+  <si>
+    <t>author_name</t>
+  </si>
+  <si>
+    <t>测试群组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_count</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>notification</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>scheduled_notification</t>
+  </si>
+  <si>
+    <t>scheduledReleaseTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -736,6 +781,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -773,7 +825,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -788,6 +840,10 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1093,7 +1149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="U1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
@@ -2629,7 +2685,7 @@
   <dimension ref="B1:F1"/>
   <sheetViews>
     <sheetView zoomScale="302" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2652,6 +2708,248 @@
       </c>
       <c r="F1" s="3" t="s">
         <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CCD222D-78F2-FB46-92FF-378DE9EBBEAE}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="167" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" s="10">
+        <v>44688.000092592592</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C9BD69-A5DF-FE46-A120-780EC78C3D4F}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView zoomScale="284" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF13D512-2C0E-CA40-A187-2B56EBABF910}">
+  <dimension ref="B1:D2"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScale="230" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4">
+      <c r="B1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4">
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7F3389-574E-F44C-BA51-BCCCD2B89F59}">
+  <dimension ref="B1:C2"/>
+  <sheetViews>
+    <sheetView zoomScale="216" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895537DF-623E-2F45-A206-75E92B904DA9}">
+  <dimension ref="B1:C1"/>
+  <sheetViews>
+    <sheetView zoomScale="191" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C32F47-7F4D-064E-93E3-D41871E697C9}">
+  <dimension ref="B1:D1"/>
+  <sheetViews>
+    <sheetView zoomScale="230" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4">
+      <c r="B1" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#42 make tag field to taglist string with whitespace
</commit_message>
<xml_diff>
--- a/testcase/real.xlsx
+++ b/testcase/real.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LearningResources\CodeAssignment\2022Spring\SoftwareEngineering\backend\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B62680-656F-EC4D-BEA1-B0B564B8B0CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413C6EFB-C895-423D-8E4D-3A5E5D2F7A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="18000" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="16665" windowWidth="16200" windowHeight="28035" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="198">
   <si>
     <t>username</t>
   </si>
@@ -336,10 +336,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>tag1,tag2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -723,13 +719,20 @@
   </si>
   <si>
     <t>scheduledReleaseTime</t>
+  </si>
+  <si>
+    <t>tag1 tag2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isObligatory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1153,13 +1156,13 @@
       <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="4"/>
-    <col min="4" max="4" width="7.1640625" style="4" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" style="4" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.875" style="4"/>
+    <col min="4" max="4" width="7.125" style="4" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="18.875" style="4" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="4" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="4" customWidth="1"/>
     <col min="8" max="8" width="26" style="4" hidden="1" customWidth="1"/>
@@ -1168,22 +1171,22 @@
     <col min="11" max="11" width="0" style="4" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="22.5" style="4" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="4" customWidth="1"/>
-    <col min="14" max="17" width="8.83203125" style="4"/>
-    <col min="18" max="18" width="20.6640625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="21.33203125" style="4" customWidth="1"/>
-    <col min="20" max="20" width="22.6640625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="16.33203125" style="4" customWidth="1"/>
-    <col min="22" max="22" width="21.6640625" style="4" customWidth="1"/>
-    <col min="23" max="23" width="22.83203125" style="4" customWidth="1"/>
-    <col min="24" max="24" width="23.33203125" style="4" customWidth="1"/>
-    <col min="25" max="25" width="21.1640625" style="4" customWidth="1"/>
-    <col min="26" max="26" width="17.83203125" style="4" customWidth="1"/>
-    <col min="27" max="27" width="18.6640625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="20.83203125" style="4" customWidth="1"/>
-    <col min="29" max="16384" width="8.83203125" style="4"/>
+    <col min="14" max="17" width="8.875" style="4"/>
+    <col min="18" max="18" width="20.625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="21.375" style="4" customWidth="1"/>
+    <col min="20" max="20" width="22.625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="16.375" style="4" customWidth="1"/>
+    <col min="22" max="22" width="21.625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="22.875" style="4" customWidth="1"/>
+    <col min="24" max="24" width="23.375" style="4" customWidth="1"/>
+    <col min="25" max="25" width="21.125" style="4" customWidth="1"/>
+    <col min="26" max="26" width="17.875" style="4" customWidth="1"/>
+    <col min="27" max="27" width="18.625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="20.875" style="4" customWidth="1"/>
+    <col min="29" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1">
+    <row r="1" spans="1:28" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1239,7 +1242,7 @@
         <v>17</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>18</v>
@@ -1269,27 +1272,27 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>80</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>77</v>
@@ -1301,7 +1304,7 @@
         <v>68</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>72</v>
@@ -1319,13 +1322,13 @@
         <v>1</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="U2" s="4">
         <v>0</v>
@@ -1334,45 +1337,45 @@
         <v>78</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>78</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Z2" s="4" t="s">
         <v>78</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AB2" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>81</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>77</v>
@@ -1384,7 +1387,7 @@
         <v>68</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>77</v>
@@ -1402,13 +1405,13 @@
         <v>1</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>77</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U3" s="4">
         <v>0</v>
@@ -1417,45 +1420,45 @@
         <v>0</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X3" s="4" t="s">
         <v>72</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Z3" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA3" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB3" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>82</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>77</v>
@@ -1467,10 +1470,10 @@
         <v>68</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>71</v>
@@ -1485,13 +1488,13 @@
         <v>1</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U4" s="4">
         <v>0</v>
@@ -1500,45 +1503,45 @@
         <v>0</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X4" s="4" t="s">
         <v>78</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Z4" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA4" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB4" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>77</v>
@@ -1553,7 +1556,7 @@
         <v>73</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>71</v>
@@ -1568,13 +1571,13 @@
         <v>1</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U5" s="4">
         <v>0</v>
@@ -1583,45 +1586,45 @@
         <v>0</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X5" s="4" t="s">
         <v>72</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Z5" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA5" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB5" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>82</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>77</v>
@@ -1633,7 +1636,7 @@
         <v>68</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>72</v>
@@ -1651,13 +1654,13 @@
         <v>1</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S6" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="U6" s="4">
         <v>0</v>
@@ -1666,45 +1669,45 @@
         <v>0</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X6" s="4" t="s">
         <v>78</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z6" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA6" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB6" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>87</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>77</v>
@@ -1716,7 +1719,7 @@
         <v>68</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>77</v>
@@ -1734,13 +1737,13 @@
         <v>1</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S7" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U7" s="4">
         <v>0</v>
@@ -1749,45 +1752,45 @@
         <v>0</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X7" s="4" t="s">
         <v>72</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Z7" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA7" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB7" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>87</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>77</v>
@@ -1802,7 +1805,7 @@
         <v>74</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>71</v>
@@ -1817,13 +1820,13 @@
         <v>1</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S8" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U8" s="4">
         <v>0</v>
@@ -1832,45 +1835,45 @@
         <v>0</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X8" s="4" t="s">
         <v>72</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Z8" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA8" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB8" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>87</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>77</v>
@@ -1882,10 +1885,10 @@
         <v>68</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>71</v>
@@ -1900,13 +1903,13 @@
         <v>1</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U9" s="4">
         <v>0</v>
@@ -1915,45 +1918,45 @@
         <v>0</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X9" s="4" t="s">
         <v>71</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Z9" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA9" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB9" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>88</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>77</v>
@@ -1965,7 +1968,7 @@
         <v>68</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>72</v>
@@ -1983,13 +1986,13 @@
         <v>1</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S10" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U10" s="4">
         <v>0</v>
@@ -1998,45 +2001,45 @@
         <v>0</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X10" s="4" t="s">
         <v>71</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Z10" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA10" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB10" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>88</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>77</v>
@@ -2066,13 +2069,13 @@
         <v>1</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S11" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U11" s="4">
         <v>0</v>
@@ -2081,45 +2084,45 @@
         <v>0</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X11" s="4" t="s">
         <v>71</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Z11" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA11" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB11" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>88</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>77</v>
@@ -2131,10 +2134,10 @@
         <v>68</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>71</v>
@@ -2149,13 +2152,13 @@
         <v>1</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S12" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U12" s="4">
         <v>0</v>
@@ -2164,25 +2167,25 @@
         <v>0</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X12" s="4" t="s">
         <v>71</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Z12" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA12" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB12" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>68</v>
       </c>
@@ -2190,19 +2193,19 @@
         <v>79</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>78</v>
@@ -2211,10 +2214,10 @@
         <v>70</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>78</v>
@@ -2229,13 +2232,13 @@
         <v>78</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S13" s="4" t="s">
         <v>77</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U13" s="4" t="s">
         <v>72</v>
@@ -2244,45 +2247,45 @@
         <v>72</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X13" s="4" t="s">
         <v>78</v>
       </c>
       <c r="Y13" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Z13" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA13" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB13" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>78</v>
@@ -2309,13 +2312,13 @@
         <v>78</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S14" s="4" t="s">
         <v>77</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U14" s="4" t="s">
         <v>72</v>
@@ -2324,45 +2327,45 @@
         <v>72</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X14" s="4" t="s">
         <v>78</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Z14" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA14" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AB14" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>78</v>
@@ -2371,7 +2374,7 @@
         <v>70</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>77</v>
@@ -2389,13 +2392,13 @@
         <v>78</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S15" s="4" t="s">
         <v>77</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U15" s="4" t="s">
         <v>72</v>
@@ -2404,45 +2407,45 @@
         <v>72</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X15" s="4" t="s">
         <v>78</v>
       </c>
       <c r="Y15" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Z15" s="4" t="s">
         <v>78</v>
       </c>
       <c r="AA15" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AB15" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>78</v>
@@ -2451,10 +2454,10 @@
         <v>70</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>72</v>
@@ -2469,13 +2472,13 @@
         <v>78</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S16" s="4" t="s">
         <v>72</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U16" s="4" t="s">
         <v>72</v>
@@ -2484,19 +2487,19 @@
         <v>72</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X16" s="4" t="s">
         <v>72</v>
       </c>
       <c r="Y16" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z16" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AA16" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AB16" s="4" t="s">
         <v>78</v>
@@ -2534,14 +2537,14 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="4"/>
-    <col min="4" max="4" width="21.33203125" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="3" width="8.875" style="4"/>
+    <col min="4" max="4" width="21.375" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="6" customFormat="1">
+    <row r="1" spans="2:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -2584,21 +2587,21 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="4"/>
-    <col min="4" max="4" width="7.83203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="4"/>
-    <col min="7" max="7" width="11.33203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="4"/>
-    <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="3" width="8.875" style="4"/>
+    <col min="4" max="4" width="7.875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="4"/>
+    <col min="7" max="7" width="11.375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="4"/>
+    <col min="9" max="9" width="17.625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.375" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="6" customFormat="1">
+    <row r="1" spans="2:12" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>62</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>66</v>
@@ -2633,44 +2636,44 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="7"/>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B20" s="7"/>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.15">
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
@@ -2688,12 +2691,12 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="6" customFormat="1">
+    <row r="1" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -2720,31 +2723,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CCD222D-78F2-FB46-92FF-378DE9EBBEAE}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="167" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="167" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="3" max="3" width="17.625" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>35</v>
@@ -2753,7 +2756,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2764,10 +2767,10 @@
         <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F2" s="10">
         <v>44688.000092592592</v>
@@ -2787,32 +2790,32 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
         <v>68</v>
@@ -2835,26 +2838,26 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.625" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B1" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2877,19 +2880,19 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="2:3">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B1" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2909,17 +2912,17 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" width="38.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B1" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2936,20 +2939,20 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B1" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2966,9 +2969,9 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1">
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
@@ -2982,40 +2985,40 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B5">
         <v>0</v>
       </c>
@@ -3023,10 +3026,10 @@
         <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B6">
         <v>1</v>
       </c>
@@ -3034,10 +3037,10 @@
         <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B7">
         <v>2</v>
       </c>
@@ -3045,7 +3048,7 @@
         <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3062,16 +3065,16 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.875" customWidth="1"/>
+    <col min="6" max="6" width="15.875" customWidth="1"/>
+    <col min="7" max="7" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="1" customFormat="1">
+    <row r="1" spans="2:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
@@ -3091,30 +3094,30 @@
         <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9">
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F2">
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -3137,13 +3140,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1">
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
@@ -3169,24 +3172,24 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView zoomScale="194" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="1" max="3" width="8.875" style="4"/>
     <col min="4" max="4" width="15" style="4" customWidth="1"/>
     <col min="5" max="5" width="12" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="4" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="4"/>
-    <col min="10" max="10" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="4"/>
+    <col min="6" max="6" width="18.625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.625" style="4" customWidth="1"/>
+    <col min="8" max="9" width="8.875" style="4"/>
+    <col min="10" max="10" width="18.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -3216,10 +3219,10 @@
         <v>44</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3233,10 +3236,10 @@
         <v>92</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>93</v>
+        <v>196</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G2" s="4">
         <v>400</v>
@@ -3245,13 +3248,13 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3262,13 +3265,13 @@
         <v>68</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G3" s="4">
         <v>4000</v>
@@ -3277,7 +3280,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>78</v>
@@ -3286,30 +3289,31 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView zoomScale="168" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="168" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="6" max="6" width="20.33203125" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.375" customWidth="1"/>
+    <col min="10" max="10" width="15.375" customWidth="1"/>
+    <col min="11" max="11" width="19.375" customWidth="1"/>
     <col min="12" max="12" width="15.5" style="4" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="15" width="8.83203125" style="4"/>
+    <col min="14" max="15" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -3363,12 +3367,16 @@
         <v>53</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3380,17 +3388,17 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="4"/>
+    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="6" max="6" width="20.875" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -3428,14 +3436,14 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="6" max="6" width="8.83203125" style="4"/>
+    <col min="6" max="6" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>54</v>
@@ -3470,12 +3478,12 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="6" customFormat="1">
+    <row r="1" spans="2:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>57</v>
       </c>
@@ -3483,7 +3491,7 @@
         <v>35</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#49 just merge from notification
</commit_message>
<xml_diff>
--- a/testcase/real.xlsx
+++ b/testcase/real.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LearningResources\CodeAssignment\2022Spring\SoftwareEngineering\backend\testcase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413C6EFB-C895-423D-8E4D-3A5E5D2F7A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5451667-18ED-3F47-87A1-EBB2A6293CFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="16665" windowWidth="16200" windowHeight="28035" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="198">
   <si>
     <t>username</t>
   </si>
@@ -732,7 +732,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1152,41 +1152,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB16"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="14.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="7.125" style="4" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="18.875" style="4" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="4" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="4" customWidth="1"/>
-    <col min="8" max="8" width="26" style="4" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="11" style="4" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="4" customWidth="1"/>
     <col min="10" max="10" width="14" style="4" customWidth="1"/>
-    <col min="11" max="11" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="22.5" style="4" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="8.1640625" style="4" customWidth="1"/>
     <col min="13" max="13" width="13" style="4" customWidth="1"/>
-    <col min="14" max="17" width="8.875" style="4"/>
-    <col min="18" max="18" width="20.625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="21.375" style="4" customWidth="1"/>
-    <col min="20" max="20" width="22.625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="16.375" style="4" customWidth="1"/>
-    <col min="22" max="22" width="21.625" style="4" customWidth="1"/>
-    <col min="23" max="23" width="22.875" style="4" customWidth="1"/>
-    <col min="24" max="24" width="23.375" style="4" customWidth="1"/>
-    <col min="25" max="25" width="21.125" style="4" customWidth="1"/>
-    <col min="26" max="26" width="17.875" style="4" customWidth="1"/>
-    <col min="27" max="27" width="18.625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="20.875" style="4" customWidth="1"/>
-    <col min="29" max="16384" width="8.875" style="4"/>
+    <col min="14" max="17" width="8.83203125" style="4"/>
+    <col min="18" max="18" width="20.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="22.6640625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="16.33203125" style="4" customWidth="1"/>
+    <col min="22" max="22" width="21.6640625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="22.83203125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="23.33203125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="21.1640625" style="4" customWidth="1"/>
+    <col min="26" max="26" width="17.83203125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="18.6640625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="20.83203125" style="4" customWidth="1"/>
+    <col min="29" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="6" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1272,7 +1271,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28">
       <c r="A2" s="4" t="s">
         <v>126</v>
       </c>
@@ -1355,7 +1354,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28">
       <c r="A3" s="4" t="s">
         <v>127</v>
       </c>
@@ -1438,7 +1437,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28">
       <c r="A4" s="4" t="s">
         <v>128</v>
       </c>
@@ -1521,7 +1520,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28">
       <c r="A5" s="4" t="s">
         <v>129</v>
       </c>
@@ -1604,7 +1603,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28">
       <c r="A6" s="4" t="s">
         <v>130</v>
       </c>
@@ -1687,7 +1686,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28">
       <c r="A7" s="4" t="s">
         <v>131</v>
       </c>
@@ -1770,7 +1769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28">
       <c r="A8" s="4" t="s">
         <v>132</v>
       </c>
@@ -1853,7 +1852,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28">
       <c r="A9" s="4" t="s">
         <v>134</v>
       </c>
@@ -1936,7 +1935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28">
       <c r="A10" s="4" t="s">
         <v>133</v>
       </c>
@@ -2019,7 +2018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:28">
       <c r="A11" s="4" t="s">
         <v>135</v>
       </c>
@@ -2102,7 +2101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:28">
       <c r="A12" s="4" t="s">
         <v>136</v>
       </c>
@@ -2185,7 +2184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:28">
       <c r="A13" s="4" t="s">
         <v>68</v>
       </c>
@@ -2213,6 +2212,9 @@
       <c r="J13" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="K13" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="L13" s="4" t="s">
         <v>172</v>
       </c>
@@ -2265,7 +2267,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28">
       <c r="A14" s="4" t="s">
         <v>98</v>
       </c>
@@ -2293,6 +2295,9 @@
       <c r="J14" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="K14" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="L14" s="4" t="s">
         <v>76</v>
       </c>
@@ -2345,7 +2350,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:28">
       <c r="A15" s="4" t="s">
         <v>99</v>
       </c>
@@ -2373,6 +2378,9 @@
       <c r="J15" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="K15" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="L15" s="4" t="s">
         <v>166</v>
       </c>
@@ -2425,7 +2433,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28">
       <c r="A16" s="4" t="s">
         <v>100</v>
       </c>
@@ -2452,6 +2460,9 @@
       </c>
       <c r="J16" s="4" t="s">
         <v>70</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>173</v>
@@ -2537,14 +2548,14 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="21.375" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.875" style="4"/>
+    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="21.33203125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -2587,21 +2598,21 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="7.875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="4"/>
-    <col min="7" max="7" width="11.375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="4"/>
-    <col min="9" max="9" width="17.625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="21.375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="13.375" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="8.875" style="4"/>
+    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="7.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="4"/>
+    <col min="7" max="7" width="11.33203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="4"/>
+    <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -2636,44 +2647,44 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:12">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:12">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:12">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:12">
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:4">
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:4">
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:4">
       <c r="B19" s="7"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:4">
       <c r="B20" s="7"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:4">
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:4">
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:4">
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:4">
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:4">
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
@@ -2691,12 +2702,12 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="16384" width="8.875" style="4"/>
+    <col min="1" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -2727,16 +2738,16 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="2" width="21.625" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
-    <col min="4" max="4" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="14.375" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -2756,7 +2767,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2790,13 +2801,13 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -2810,7 +2821,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2838,13 +2849,13 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="3" max="3" width="26.625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:4">
       <c r="B1" s="11" t="s">
         <v>58</v>
       </c>
@@ -2855,7 +2866,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:4">
       <c r="B2" t="s">
         <v>100</v>
       </c>
@@ -2880,9 +2891,9 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:3">
       <c r="B1" s="11" t="s">
         <v>58</v>
       </c>
@@ -2890,7 +2901,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:3">
       <c r="B2" t="s">
         <v>100</v>
       </c>
@@ -2912,12 +2923,12 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="3" max="3" width="38.625" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:3">
       <c r="B1" s="11" t="s">
         <v>58</v>
       </c>
@@ -2939,12 +2950,12 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="4" max="4" width="27.625" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:4">
       <c r="B1" s="11" t="s">
         <v>186</v>
       </c>
@@ -2969,9 +2980,9 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" s="1" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
@@ -2985,7 +2996,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:5">
       <c r="B2">
         <v>0</v>
       </c>
@@ -2996,7 +3007,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:5">
       <c r="B3">
         <v>1</v>
       </c>
@@ -3007,7 +3018,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:5">
       <c r="B4">
         <v>2</v>
       </c>
@@ -3018,7 +3029,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:5">
       <c r="B5">
         <v>0</v>
       </c>
@@ -3029,7 +3040,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:5">
       <c r="B6">
         <v>1</v>
       </c>
@@ -3040,7 +3051,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:5">
       <c r="B7">
         <v>2</v>
       </c>
@@ -3065,16 +3076,16 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="14.875" customWidth="1"/>
-    <col min="6" max="6" width="15.875" customWidth="1"/>
-    <col min="7" max="7" width="20.125" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" s="1" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
@@ -3100,7 +3111,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:9">
       <c r="B2" t="s">
         <v>126</v>
       </c>
@@ -3140,13 +3151,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" s="1" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
@@ -3175,19 +3186,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
+    <col min="1" max="3" width="8.83203125" style="4"/>
     <col min="4" max="4" width="15" style="4" customWidth="1"/>
     <col min="5" max="5" width="12" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20.625" style="4" customWidth="1"/>
-    <col min="8" max="9" width="8.875" style="4"/>
-    <col min="10" max="10" width="18.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.875" style="4"/>
+    <col min="6" max="6" width="18.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="4" customWidth="1"/>
+    <col min="8" max="9" width="8.83203125" style="4"/>
+    <col min="10" max="10" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>93</v>
       </c>
@@ -3222,7 +3233,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3254,7 +3265,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3297,21 +3308,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="168" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="N1" zoomScale="168" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="6" max="6" width="20.375" customWidth="1"/>
-    <col min="10" max="10" width="15.375" customWidth="1"/>
-    <col min="11" max="11" width="19.375" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
     <col min="12" max="12" width="15.5" style="4" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="15" width="8.875" style="4"/>
+    <col min="14" max="15" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>93</v>
       </c>
@@ -3388,15 +3399,15 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
-    <col min="6" max="6" width="20.875" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="4"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>93</v>
       </c>
@@ -3436,12 +3447,12 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="6" max="6" width="8.875" style="4"/>
+    <col min="6" max="6" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>93</v>
       </c>
@@ -3478,12 +3489,12 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="16384" width="8.875" style="4"/>
+    <col min="1" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
#57 Notification system made more robust with new database info
</commit_message>
<xml_diff>
--- a/testcase/real.xlsx
+++ b/testcase/real.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LearningResources\CodeAssignment\2022Spring\SoftwareEngineering\backend\testcase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archive\Personal\code\SE\backend\backend\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413C6EFB-C895-423D-8E4D-3A5E5D2F7A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2458CB-AFC1-47C3-8A9F-2E8140926AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="16665" windowWidth="16200" windowHeight="28035" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="199">
   <si>
     <t>username</t>
   </si>
@@ -726,6 +726,10 @@
   </si>
   <si>
     <t>isObligatory</t>
+  </si>
+  <si>
+    <t>author_username</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -800,7 +804,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -823,12 +827,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -845,6 +860,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2721,10 +2739,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CCD222D-78F2-FB46-92FF-378DE9EBBEAE}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="167" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="167" workbookViewId="0">
+      <selection activeCell="I9" activeCellId="1" sqref="G1:G2 I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2734,9 +2752,10 @@
     <col min="4" max="4" width="12.625" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
     <col min="6" max="6" width="14.375" customWidth="1"/>
+    <col min="7" max="7" width="16.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -2755,8 +2774,11 @@
       <c r="F1" s="11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G1" s="12" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2774,6 +2796,9 @@
       </c>
       <c r="F2" s="10">
         <v>44688.000092592592</v>
+      </c>
+      <c r="G2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3297,7 +3322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="168" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="N1" zoomScale="168" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>

</xml_diff>